<commit_message>
change docs and code
</commit_message>
<xml_diff>
--- a/docs/прочее/students.xlsx
+++ b/docs/прочее/students.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Диплом\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\diplom-app\docs\прочее\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BC5033-DFF7-4DD6-80E5-A2C4A0EE6F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D9D104-9B3F-4C55-94E6-DDC7354FD6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
     <t>firstName</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>Александрович</t>
+  </si>
+  <si>
+    <t>faculty</t>
+  </si>
+  <si>
+    <t>group</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,12 +575,12 @@
     <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="21.140625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,8 +605,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -616,22 +628,30 @@
       </c>
       <c r="E2">
         <f ca="1" xml:space="preserve"> INT(RAND() * 12345678)</f>
-        <v>5660612</v>
+        <v>672367</v>
       </c>
       <c r="F2">
         <f ca="1">INT(RAND() * 12) + 3</f>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G2">
         <f ca="1">INT(RAND() * 8) + 1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H2">
         <f ca="1">INT(RAND() * 2) + 1</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I2" t="str">
+        <f ca="1">IF(RAND() &gt; 0.5, "ФАИС","ЭФ")</f>
+        <v>ЭФ</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">IF(RAND() &gt; 0.5, "ИП-42","ИТИ-21")</f>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -642,27 +662,35 @@
         <v>9</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D21" ca="1" si="0">IF(RAND() &gt; 0.5, "платное","бесплатное")</f>
+        <f ca="1">IF(RAND() &gt; 0.5, "платное","бесплатное")</f>
         <v>бесплатное</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E21" ca="1" si="1" xml:space="preserve"> INT(RAND() * 12345678)</f>
-        <v>4581345</v>
+        <f t="shared" ref="E3:E21" ca="1" si="0" xml:space="preserve"> INT(RAND() * 12345678)</f>
+        <v>10913425</v>
       </c>
       <c r="F3">
         <f ca="1">INT(RAND() * 10) + 3</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G21" ca="1" si="2">INT(RAND() * 8) + 1</f>
-        <v>6</v>
+        <f t="shared" ref="G3:G21" ca="1" si="1">INT(RAND() * 8) + 1</f>
+        <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H21" ca="1" si="3">INT(RAND() * 2) + 1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H3:H21" ca="1" si="2">INT(RAND() * 2) + 1</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I21" ca="1" si="3">IF(RAND() &gt; 0.5, "ФАИС","ЭФ")</f>
+        <v>ФАИС</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J21" ca="1" si="4">IF(RAND() &gt; 0.5, "ИП-42","ИТИ-21")</f>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -673,27 +701,35 @@
         <v>10</v>
       </c>
       <c r="D4" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>бесплатное</v>
+        <f t="shared" ref="D3:D21" ca="1" si="5">IF(RAND() &gt; 0.5, "платное","бесплатное")</f>
+        <v>платное</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="1"/>
-        <v>5363035</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6852264</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F21" ca="1" si="4">INT(RAND() * 14) + 3</f>
-        <v>10</v>
+        <f t="shared" ref="F4:F21" ca="1" si="6">INT(RAND() * 14) + 3</f>
+        <v>5</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>6</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>31</v>
       </c>
@@ -704,27 +740,35 @@
         <v>11</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>бесплатное</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>платное</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="1"/>
-        <v>331464</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7847717</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I5" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -735,27 +779,35 @@
         <v>12</v>
       </c>
       <c r="D6" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>платное</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="1"/>
-        <v>4454094</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>83731</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>11</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I6" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
@@ -766,27 +818,35 @@
         <v>13</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1861619</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9062041</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>5</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -797,27 +857,35 @@
         <v>14</v>
       </c>
       <c r="D8" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="1"/>
-        <v>8257085</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6731019</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I8" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>35</v>
       </c>
@@ -828,27 +896,35 @@
         <v>15</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>бесплатное</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>платное</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="1"/>
-        <v>10732063</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6624215</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
         <v>7</v>
       </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
       <c r="H9">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -859,27 +935,35 @@
         <v>16</v>
       </c>
       <c r="D10" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>12057520</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11844132</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="4"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>15</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -890,27 +974,35 @@
         <v>17</v>
       </c>
       <c r="D11" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>платное</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="1"/>
-        <v>5144376</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2907482</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -921,27 +1013,35 @@
         <v>18</v>
       </c>
       <c r="D12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>платное</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>бесплатное</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="1"/>
-        <v>4068118</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2741213</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>16</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I12" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -952,27 +1052,35 @@
         <v>19</v>
       </c>
       <c r="D13" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>2802520</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9103432</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>16</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -983,27 +1091,35 @@
         <v>20</v>
       </c>
       <c r="D14" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="1"/>
-        <v>5408866</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6547976</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1014,27 +1130,35 @@
         <v>21</v>
       </c>
       <c r="D15" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="1"/>
-        <v>3251216</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7284702</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>12</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1045,27 +1169,35 @@
         <v>22</v>
       </c>
       <c r="D16" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>платное</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="1"/>
-        <v>1541084</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11812920</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1076,27 +1208,35 @@
         <v>23</v>
       </c>
       <c r="D17" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="1"/>
-        <v>6353395</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10800755</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1107,27 +1247,35 @@
         <v>24</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>платное</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>бесплатное</v>
       </c>
       <c r="E18">
-        <f t="shared" ca="1" si="1"/>
-        <v>1358065</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7176876</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>14</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I18" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
@@ -1138,27 +1286,35 @@
         <v>25</v>
       </c>
       <c r="D19" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="1"/>
-        <v>3076531</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4250361</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИП-42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
@@ -1169,27 +1325,35 @@
         <v>26</v>
       </c>
       <c r="D20" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="1"/>
-        <v>6285266</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7305892</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ФАИС</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -1200,24 +1364,32 @@
         <v>27</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="5"/>
         <v>бесплатное</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="1"/>
-        <v>6256528</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9161654</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="6"/>
         <v>5</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="2"/>
         <v>2</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>ЭФ</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>ИТИ-21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>